<commit_message>
POO et métriques de risque
</commit_message>
<xml_diff>
--- a/Data/Poids des entreprises dans le CAC40.xlsx
+++ b/Data/Poids des entreprises dans le CAC40.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Billn\Documents\M2QF\Cutting edge\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Billn\Documents\M2QF\Cutting edge\Cutting-edge\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EB52FE3E-467F-42AF-A7D1-4C907C75A30D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A96211DA-8055-4005-8EE7-D95583522AC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{318143BF-5913-4B99-BA51-A13E97792330}"/>
   </bookViews>
@@ -218,11 +218,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -557,10 +561,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E76D879E-1FE8-4F9A-B968-15F83995A338}">
-  <dimension ref="A1:AO2"/>
+  <dimension ref="A1:AO5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -573,124 +577,124 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" t="s">
+        <v>39</v>
+      </c>
+      <c r="L1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>9</v>
+      </c>
+      <c r="R1" t="s">
+        <v>38</v>
+      </c>
+      <c r="S1" t="s">
+        <v>3</v>
+      </c>
+      <c r="T1" t="s">
+        <v>24</v>
+      </c>
+      <c r="U1" t="s">
+        <v>25</v>
+      </c>
+      <c r="V1" t="s">
+        <v>4</v>
+      </c>
+      <c r="W1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="X1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AE1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="AF1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AL1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" t="s">
-        <v>9</v>
-      </c>
-      <c r="J1" t="s">
-        <v>10</v>
-      </c>
-      <c r="K1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L1" t="s">
-        <v>12</v>
-      </c>
-      <c r="M1" t="s">
-        <v>13</v>
-      </c>
-      <c r="N1" t="s">
+      <c r="AM1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AO1" t="s">
         <v>14</v>
-      </c>
-      <c r="O1" t="s">
-        <v>15</v>
-      </c>
-      <c r="P1" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>17</v>
-      </c>
-      <c r="R1" t="s">
-        <v>18</v>
-      </c>
-      <c r="S1" t="s">
-        <v>19</v>
-      </c>
-      <c r="T1" t="s">
-        <v>20</v>
-      </c>
-      <c r="U1" t="s">
-        <v>21</v>
-      </c>
-      <c r="V1" t="s">
-        <v>22</v>
-      </c>
-      <c r="W1" t="s">
-        <v>23</v>
-      </c>
-      <c r="X1" t="s">
-        <v>24</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>25</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>32</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>33</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>34</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>35</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>37</v>
-      </c>
-      <c r="AL1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AM1" t="s">
-        <v>39</v>
-      </c>
-      <c r="AN1" t="s">
-        <v>40</v>
-      </c>
-      <c r="AO1" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:41" x14ac:dyDescent="0.25">
@@ -698,127 +702,142 @@
         <v>1</v>
       </c>
       <c r="B2">
+        <v>4.3986803958812361E-3</v>
+      </c>
+      <c r="C2">
+        <v>5.1884434669599126E-2</v>
+      </c>
+      <c r="D2">
+        <v>4.0387883634909527E-2</v>
+      </c>
+      <c r="E2">
+        <v>9.1972408277516751E-3</v>
+      </c>
+      <c r="F2">
+        <v>3.3090072978106566E-2</v>
+      </c>
+      <c r="G2">
+        <v>3.358992302309307E-2</v>
+      </c>
+      <c r="H2">
+        <v>5.198440467859642E-3</v>
+      </c>
+      <c r="I2">
+        <v>5.0984704588623421E-3</v>
+      </c>
+      <c r="J2">
+        <v>1.0096970908727382E-2</v>
+      </c>
+      <c r="K2">
+        <v>3.2990102969109266E-3</v>
+      </c>
+      <c r="L2">
+        <v>1.9494151754473658E-2</v>
+      </c>
+      <c r="M2">
+        <v>1.7994601619514144E-2</v>
+      </c>
+      <c r="N2">
+        <v>1.9994001799460162E-2</v>
+      </c>
+      <c r="O2">
+        <v>3.1990402879136263E-3</v>
+      </c>
+      <c r="P2">
+        <v>1.5795261421573531E-2</v>
+      </c>
+      <c r="Q2">
+        <v>4.8185544336698992E-2</v>
+      </c>
+      <c r="R2">
+        <v>3.6988903329001305E-3</v>
+      </c>
+      <c r="S2">
+        <v>0.10276916924922525</v>
+      </c>
+      <c r="T2">
+        <v>1.1896431070678797E-2</v>
+      </c>
+      <c r="U2">
+        <v>1.0796760971708489E-2</v>
+      </c>
+      <c r="V2">
+        <v>7.4577626711986408E-2</v>
+      </c>
+      <c r="W2">
         <v>0.1230630810756773</v>
       </c>
-      <c r="C2">
-        <v>0.10276916924922525</v>
-      </c>
-      <c r="D2">
-        <v>7.4577626711986408E-2</v>
-      </c>
-      <c r="E2">
+      <c r="X2">
+        <v>9.5971208637408763E-3</v>
+      </c>
+      <c r="Y2">
+        <v>1.2096371088673398E-2</v>
+      </c>
+      <c r="Z2">
+        <v>9.997000899730081E-3</v>
+      </c>
+      <c r="AA2">
+        <v>9.1972408277516751E-3</v>
+      </c>
+      <c r="AB2">
+        <v>5.3983804858542444E-3</v>
+      </c>
+      <c r="AC2">
+        <v>4.0487853643906828E-2</v>
+      </c>
+      <c r="AD2">
+        <v>2.0393881835449369E-2</v>
+      </c>
+      <c r="AE2">
         <v>5.3383984804558637E-2</v>
       </c>
-      <c r="F2">
-        <v>5.1884434669599126E-2</v>
-      </c>
-      <c r="G2">
+      <c r="AF2">
+        <v>4.8785364390682803E-2</v>
+      </c>
+      <c r="AG2">
+        <v>1.2996101169649105E-2</v>
+      </c>
+      <c r="AH2">
+        <v>1.2996101169649105E-2</v>
+      </c>
+      <c r="AI2">
+        <v>8.2975107467759667E-3</v>
+      </c>
+      <c r="AJ2">
+        <v>2.3992802159352191E-3</v>
+      </c>
+      <c r="AK2">
+        <v>1.8894331700489854E-2</v>
+      </c>
+      <c r="AL2">
         <v>4.8985304408677398E-2</v>
       </c>
-      <c r="H2">
-        <v>4.8785364390682803E-2</v>
-      </c>
-      <c r="I2">
-        <v>4.8185544336698992E-2</v>
-      </c>
-      <c r="J2">
-        <v>4.0487853643906828E-2</v>
-      </c>
-      <c r="K2">
-        <v>4.0387883634909527E-2</v>
-      </c>
-      <c r="L2">
-        <v>3.358992302309307E-2</v>
-      </c>
-      <c r="M2">
-        <v>3.3090072978106566E-2</v>
-      </c>
-      <c r="N2">
+      <c r="AM2">
+        <v>4.1987403778866337E-3</v>
+      </c>
+      <c r="AN2">
+        <v>8.6973907827651697E-3</v>
+      </c>
+      <c r="AO2">
         <v>2.5492352294311706E-2</v>
       </c>
-      <c r="O2">
-        <v>2.0393881835449369E-2</v>
-      </c>
-      <c r="P2">
-        <v>1.9994001799460162E-2</v>
-      </c>
-      <c r="Q2">
-        <v>1.9494151754473658E-2</v>
-      </c>
-      <c r="R2">
-        <v>1.8894331700489854E-2</v>
-      </c>
-      <c r="S2">
-        <v>1.7994601619514144E-2</v>
-      </c>
-      <c r="T2">
-        <v>1.5795261421573531E-2</v>
-      </c>
-      <c r="U2">
-        <v>1.2996101169649105E-2</v>
-      </c>
-      <c r="V2">
-        <v>1.2996101169649105E-2</v>
-      </c>
-      <c r="W2">
-        <v>1.2096371088673398E-2</v>
-      </c>
-      <c r="X2">
-        <v>1.1896431070678797E-2</v>
-      </c>
-      <c r="Y2">
-        <v>1.0796760971708489E-2</v>
-      </c>
-      <c r="Z2">
-        <v>1.0096970908727382E-2</v>
-      </c>
-      <c r="AA2">
-        <v>9.997000899730081E-3</v>
-      </c>
-      <c r="AB2">
-        <v>9.5971208637408763E-3</v>
-      </c>
-      <c r="AC2">
-        <v>9.1972408277516751E-3</v>
-      </c>
-      <c r="AD2">
-        <v>9.1972408277516751E-3</v>
-      </c>
-      <c r="AE2">
-        <v>8.6973907827651697E-3</v>
-      </c>
-      <c r="AF2">
-        <v>8.2975107467759667E-3</v>
-      </c>
-      <c r="AG2">
-        <v>5.3983804858542444E-3</v>
-      </c>
-      <c r="AH2">
-        <v>5.198440467859642E-3</v>
-      </c>
-      <c r="AI2">
-        <v>5.0984704588623421E-3</v>
-      </c>
-      <c r="AJ2">
-        <v>4.3986803958812361E-3</v>
-      </c>
-      <c r="AK2">
-        <v>4.1987403778866337E-3</v>
-      </c>
-      <c r="AL2">
-        <v>3.6988903329001305E-3</v>
-      </c>
-      <c r="AM2">
-        <v>3.2990102969109266E-3</v>
-      </c>
-      <c r="AN2">
-        <v>3.1990402879136263E-3</v>
-      </c>
-      <c r="AO2">
-        <v>2.3992802159352191E-3</v>
-      </c>
+    </row>
+    <row r="3" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+      <c r="B3" s="3"/>
+    </row>
+    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+    </row>
+    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:B44">
+    <sortCondition ref="A5:A44"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>